<commit_message>
Rutas Player protegidas usando Passport y JWT. Podría agregarlas a Delete y Update de Users....
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BC2"/>
+  <dimension ref="A1:BC6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -733,9 +733,665 @@
         <v>Finesse Shot, Speed Dribbler (AI), One Club Player, Team Player</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>15</v>
+      </c>
+      <c r="C3" t="str">
+        <v>2</v>
+      </c>
+      <c r="D3" t="str">
+        <v>https://cdn.sofifa.net/players/020/801/15_120.png</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Cristiano Ronaldo dos Santos Aveiro</v>
+      </c>
+      <c r="F3" t="str">
+        <v>LW, LM</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Real Madrid CF</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Portugal</v>
+      </c>
+      <c r="I3">
+        <v>92</v>
+      </c>
+      <c r="J3">
+        <v>92</v>
+      </c>
+      <c r="K3">
+        <v>79000000</v>
+      </c>
+      <c r="L3">
+        <v>375000</v>
+      </c>
+      <c r="M3">
+        <v>29</v>
+      </c>
+      <c r="N3">
+        <v>185</v>
+      </c>
+      <c r="O3">
+        <v>80</v>
+      </c>
+      <c r="P3" t="str">
+        <v>Right</v>
+      </c>
+      <c r="Q3">
+        <v>4</v>
+      </c>
+      <c r="R3">
+        <v>5</v>
+      </c>
+      <c r="S3">
+        <v>5</v>
+      </c>
+      <c r="T3" t="str">
+        <v>High/Low</v>
+      </c>
+      <c r="U3" t="str">
+        <v>Normal (185+)</v>
+      </c>
+      <c r="V3">
+        <v>93</v>
+      </c>
+      <c r="W3">
+        <v>93</v>
+      </c>
+      <c r="X3">
+        <v>81</v>
+      </c>
+      <c r="Y3">
+        <v>91</v>
+      </c>
+      <c r="Z3">
+        <v>88</v>
+      </c>
+      <c r="AA3">
+        <v>79</v>
+      </c>
+      <c r="AB3">
+        <v>72</v>
+      </c>
+      <c r="AC3">
+        <v>92</v>
+      </c>
+      <c r="AD3">
+        <v>91</v>
+      </c>
+      <c r="AE3">
+        <v>94</v>
+      </c>
+      <c r="AF3">
+        <v>93</v>
+      </c>
+      <c r="AG3">
+        <v>90</v>
+      </c>
+      <c r="AH3">
+        <v>63</v>
+      </c>
+      <c r="AI3">
+        <v>94</v>
+      </c>
+      <c r="AJ3">
+        <v>94</v>
+      </c>
+      <c r="AK3">
+        <v>89</v>
+      </c>
+      <c r="AL3">
+        <v>79</v>
+      </c>
+      <c r="AM3">
+        <v>93</v>
+      </c>
+      <c r="AN3">
+        <v>63</v>
+      </c>
+      <c r="AO3">
+        <v>24</v>
+      </c>
+      <c r="AP3">
+        <v>91</v>
+      </c>
+      <c r="AQ3">
+        <v>81</v>
+      </c>
+      <c r="AR3">
+        <v>85</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AU3">
+        <v>31</v>
+      </c>
+      <c r="AV3">
+        <v>23</v>
+      </c>
+      <c r="AW3">
+        <v>7</v>
+      </c>
+      <c r="AX3">
+        <v>11</v>
+      </c>
+      <c r="AY3">
+        <v>15</v>
+      </c>
+      <c r="AZ3">
+        <v>14</v>
+      </c>
+      <c r="BA3">
+        <v>11</v>
+      </c>
+      <c r="BB3">
+        <v>0</v>
+      </c>
+      <c r="BC3" t="str">
+        <v>Power Free-Kick, Flair, Long Shot Taker (AI), Speed Dribbler (AI)</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>15</v>
+      </c>
+      <c r="C4" t="str">
+        <v>2</v>
+      </c>
+      <c r="D4" t="str">
+        <v>https://cdn.sofifa.net/players/009/014/15_120.png</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Arjen Robben</v>
+      </c>
+      <c r="F4" t="str">
+        <v>RM, LM, RW</v>
+      </c>
+      <c r="G4" t="str">
+        <v>FC Bayern München</v>
+      </c>
+      <c r="H4" t="str">
+        <v>Netherlands</v>
+      </c>
+      <c r="I4">
+        <v>90</v>
+      </c>
+      <c r="J4">
+        <v>90</v>
+      </c>
+      <c r="K4">
+        <v>54500000</v>
+      </c>
+      <c r="L4">
+        <v>275000</v>
+      </c>
+      <c r="M4">
+        <v>30</v>
+      </c>
+      <c r="N4">
+        <v>180</v>
+      </c>
+      <c r="O4">
+        <v>80</v>
+      </c>
+      <c r="P4" t="str">
+        <v>Left</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <v>4</v>
+      </c>
+      <c r="S4">
+        <v>5</v>
+      </c>
+      <c r="T4" t="str">
+        <v>High/Low</v>
+      </c>
+      <c r="U4" t="str">
+        <v>Normal (170-185)</v>
+      </c>
+      <c r="V4">
+        <v>93</v>
+      </c>
+      <c r="W4">
+        <v>86</v>
+      </c>
+      <c r="X4">
+        <v>83</v>
+      </c>
+      <c r="Y4">
+        <v>92</v>
+      </c>
+      <c r="Z4">
+        <v>85</v>
+      </c>
+      <c r="AA4">
+        <v>83</v>
+      </c>
+      <c r="AB4">
+        <v>76</v>
+      </c>
+      <c r="AC4">
+        <v>90</v>
+      </c>
+      <c r="AD4">
+        <v>93</v>
+      </c>
+      <c r="AE4">
+        <v>93</v>
+      </c>
+      <c r="AF4">
+        <v>93</v>
+      </c>
+      <c r="AG4">
+        <v>89</v>
+      </c>
+      <c r="AH4">
+        <v>91</v>
+      </c>
+      <c r="AI4">
+        <v>86</v>
+      </c>
+      <c r="AJ4">
+        <v>61</v>
+      </c>
+      <c r="AK4">
+        <v>78</v>
+      </c>
+      <c r="AL4">
+        <v>65</v>
+      </c>
+      <c r="AM4">
+        <v>90</v>
+      </c>
+      <c r="AN4">
+        <v>47</v>
+      </c>
+      <c r="AO4">
+        <v>39</v>
+      </c>
+      <c r="AP4">
+        <v>89</v>
+      </c>
+      <c r="AQ4">
+        <v>84</v>
+      </c>
+      <c r="AR4">
+        <v>80</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>26</v>
+      </c>
+      <c r="AV4">
+        <v>26</v>
+      </c>
+      <c r="AW4">
+        <v>10</v>
+      </c>
+      <c r="AX4">
+        <v>8</v>
+      </c>
+      <c r="AY4">
+        <v>11</v>
+      </c>
+      <c r="AZ4">
+        <v>5</v>
+      </c>
+      <c r="BA4">
+        <v>15</v>
+      </c>
+      <c r="BB4">
+        <v>0</v>
+      </c>
+      <c r="BC4" t="str">
+        <v>Diver, Injury Prone, Avoids Using Weaker Foot, Selfish, Long Shot Taker (AI), Speed Dribbler (AI), Chip Shot (AI)</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>15</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2</v>
+      </c>
+      <c r="D5" t="str">
+        <v>https://cdn.sofifa.net/players/041/236/15_120.png</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Zlatan Ibrahimović</v>
+      </c>
+      <c r="F5" t="str">
+        <v>ST</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Paris Saint-Germain</v>
+      </c>
+      <c r="H5" t="str">
+        <v>Sweden</v>
+      </c>
+      <c r="I5">
+        <v>90</v>
+      </c>
+      <c r="J5">
+        <v>90</v>
+      </c>
+      <c r="K5">
+        <v>52500000</v>
+      </c>
+      <c r="L5">
+        <v>275000</v>
+      </c>
+      <c r="M5">
+        <v>32</v>
+      </c>
+      <c r="N5">
+        <v>195</v>
+      </c>
+      <c r="O5">
+        <v>95</v>
+      </c>
+      <c r="P5" t="str">
+        <v>Right</v>
+      </c>
+      <c r="Q5">
+        <v>4</v>
+      </c>
+      <c r="R5">
+        <v>4</v>
+      </c>
+      <c r="S5">
+        <v>5</v>
+      </c>
+      <c r="T5" t="str">
+        <v>Medium/Low</v>
+      </c>
+      <c r="U5" t="str">
+        <v>Normal (185+)</v>
+      </c>
+      <c r="V5">
+        <v>76</v>
+      </c>
+      <c r="W5">
+        <v>91</v>
+      </c>
+      <c r="X5">
+        <v>81</v>
+      </c>
+      <c r="Y5">
+        <v>86</v>
+      </c>
+      <c r="Z5">
+        <v>80</v>
+      </c>
+      <c r="AA5">
+        <v>80</v>
+      </c>
+      <c r="AB5">
+        <v>76</v>
+      </c>
+      <c r="AC5">
+        <v>90</v>
+      </c>
+      <c r="AD5">
+        <v>74</v>
+      </c>
+      <c r="AE5">
+        <v>77</v>
+      </c>
+      <c r="AF5">
+        <v>86</v>
+      </c>
+      <c r="AG5">
+        <v>85</v>
+      </c>
+      <c r="AH5">
+        <v>41</v>
+      </c>
+      <c r="AI5">
+        <v>93</v>
+      </c>
+      <c r="AJ5">
+        <v>72</v>
+      </c>
+      <c r="AK5">
+        <v>78</v>
+      </c>
+      <c r="AL5">
+        <v>93</v>
+      </c>
+      <c r="AM5">
+        <v>88</v>
+      </c>
+      <c r="AN5">
+        <v>84</v>
+      </c>
+      <c r="AO5">
+        <v>20</v>
+      </c>
+      <c r="AP5">
+        <v>86</v>
+      </c>
+      <c r="AQ5">
+        <v>83</v>
+      </c>
+      <c r="AR5">
+        <v>91</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>41</v>
+      </c>
+      <c r="AV5">
+        <v>27</v>
+      </c>
+      <c r="AW5">
+        <v>13</v>
+      </c>
+      <c r="AX5">
+        <v>15</v>
+      </c>
+      <c r="AY5">
+        <v>10</v>
+      </c>
+      <c r="AZ5">
+        <v>9</v>
+      </c>
+      <c r="BA5">
+        <v>12</v>
+      </c>
+      <c r="BB5">
+        <v>0</v>
+      </c>
+      <c r="BC5" t="str">
+        <v>Power Free-Kick, Leadership, Flair, Long Shot Taker (AI), Technical Dribbler (AI)</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>15</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2</v>
+      </c>
+      <c r="D6" t="str">
+        <v>https://cdn.sofifa.net/players/167/495/15_120.png</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Manuel Peter Neuer</v>
+      </c>
+      <c r="F6" t="str">
+        <v>GK</v>
+      </c>
+      <c r="G6" t="str">
+        <v>FC Bayern München</v>
+      </c>
+      <c r="H6" t="str">
+        <v>Germany</v>
+      </c>
+      <c r="I6">
+        <v>90</v>
+      </c>
+      <c r="J6">
+        <v>90</v>
+      </c>
+      <c r="K6">
+        <v>63500000</v>
+      </c>
+      <c r="L6">
+        <v>300000</v>
+      </c>
+      <c r="M6">
+        <v>28</v>
+      </c>
+      <c r="N6">
+        <v>193</v>
+      </c>
+      <c r="O6">
+        <v>92</v>
+      </c>
+      <c r="P6" t="str">
+        <v>Right</v>
+      </c>
+      <c r="Q6">
+        <v>4</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>5</v>
+      </c>
+      <c r="T6" t="str">
+        <v>Medium/Medium</v>
+      </c>
+      <c r="U6" t="str">
+        <v>Normal (185+)</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>25</v>
+      </c>
+      <c r="AA6">
+        <v>25</v>
+      </c>
+      <c r="AB6">
+        <v>41</v>
+      </c>
+      <c r="AC6">
+        <v>31</v>
+      </c>
+      <c r="AD6">
+        <v>58</v>
+      </c>
+      <c r="AE6">
+        <v>61</v>
+      </c>
+      <c r="AF6">
+        <v>43</v>
+      </c>
+      <c r="AG6">
+        <v>89</v>
+      </c>
+      <c r="AH6">
+        <v>35</v>
+      </c>
+      <c r="AI6">
+        <v>42</v>
+      </c>
+      <c r="AJ6">
+        <v>78</v>
+      </c>
+      <c r="AK6">
+        <v>44</v>
+      </c>
+      <c r="AL6">
+        <v>83</v>
+      </c>
+      <c r="AM6">
+        <v>25</v>
+      </c>
+      <c r="AN6">
+        <v>29</v>
+      </c>
+      <c r="AO6">
+        <v>30</v>
+      </c>
+      <c r="AP6">
+        <v>25</v>
+      </c>
+      <c r="AQ6">
+        <v>20</v>
+      </c>
+      <c r="AR6">
+        <v>37</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>25</v>
+      </c>
+      <c r="AV6">
+        <v>25</v>
+      </c>
+      <c r="AW6">
+        <v>87</v>
+      </c>
+      <c r="AX6">
+        <v>85</v>
+      </c>
+      <c r="AY6">
+        <v>92</v>
+      </c>
+      <c r="AZ6">
+        <v>90</v>
+      </c>
+      <c r="BA6">
+        <v>86</v>
+      </c>
+      <c r="BB6">
+        <v>60</v>
+      </c>
+      <c r="BC6" t="str">
+        <v>GK Up for Corners, GK Long Throw, 1-on-1 Rush</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:BC2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:BC6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>